<commit_message>
Refactored again the import excel
</commit_message>
<xml_diff>
--- a/db_tools/acctg_db1/acctg_export1.xlsx
+++ b/db_tools/acctg_db1/acctg_export1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgrammingPython\thanos_app\db_tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgrammingPython\thanos_app\db_tools\acctg_db1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349C920D-BEAD-4864-8773-9E7498784BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914B8325-6071-4C1A-9E88-3A44BD8A50F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28665" yWindow="-135" windowWidth="29070" windowHeight="15750" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="14" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="account_types" sheetId="1" r:id="rId1"/>
@@ -2141,13 +2141,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7021,7 +7024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -7241,9 +7244,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="11" width="8.88671875" style="4"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -7270,13 +7278,13 @@
       <c r="H1" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>611</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -7305,7 +7313,7 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>1</v>
       </c>
       <c r="L2" t="s">
@@ -7334,7 +7342,7 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <v>2</v>
       </c>
       <c r="L3" t="s">
@@ -7363,7 +7371,7 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>3</v>
       </c>
       <c r="L4" t="s">
@@ -7392,7 +7400,7 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="4">
         <v>1</v>
       </c>
       <c r="L5" t="s">
@@ -7421,7 +7429,7 @@
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>4</v>
       </c>
       <c r="L6" t="s">
@@ -7450,7 +7458,7 @@
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="4">
         <v>1</v>
       </c>
       <c r="L7" t="s">
@@ -7479,7 +7487,7 @@
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <v>5</v>
       </c>
       <c r="L8" t="s">
@@ -7508,7 +7516,7 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="4">
         <v>2</v>
       </c>
       <c r="L9" t="s">
@@ -7537,7 +7545,7 @@
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="4">
         <v>2</v>
       </c>
       <c r="L10" t="s">
@@ -7566,7 +7574,7 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="4">
         <v>6</v>
       </c>
       <c r="L11" t="s">
@@ -7595,7 +7603,7 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="4">
         <v>7</v>
       </c>
       <c r="L12" t="s">
@@ -7624,7 +7632,7 @@
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="4">
         <v>8</v>
       </c>
       <c r="L13" t="s">
@@ -7653,7 +7661,7 @@
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="4">
         <v>3</v>
       </c>
       <c r="L14" t="s">
@@ -7682,7 +7690,7 @@
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="4">
         <v>3</v>
       </c>
       <c r="L15" t="s">
@@ -8391,7 +8399,7 @@
       <c r="M12" t="s">
         <v>637</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" t="s">
         <v>636</v>
       </c>
       <c r="O12" t="s">
@@ -8444,7 +8452,7 @@
       <c r="M13" t="s">
         <v>638</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="N13" t="s">
         <v>636</v>
       </c>
       <c r="O13" t="s">
@@ -8497,7 +8505,7 @@
       <c r="M14" t="s">
         <v>639</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="N14" t="s">
         <v>636</v>
       </c>
       <c r="O14" t="s">
@@ -8550,7 +8558,7 @@
       <c r="M15" t="s">
         <v>640</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="N15" t="s">
         <v>636</v>
       </c>
       <c r="O15" t="s">
@@ -8603,7 +8611,7 @@
       <c r="M16" t="s">
         <v>641</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="N16" t="s">
         <v>636</v>
       </c>
       <c r="O16" t="s">
@@ -8708,7 +8716,7 @@
       <c r="D1" t="s">
         <v>644</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>645</v>
       </c>
       <c r="F1" t="s">
@@ -8766,7 +8774,7 @@
       <c r="D3" t="s">
         <v>656</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>209268717220</v>
       </c>
       <c r="F3" t="s">
@@ -8795,7 +8803,7 @@
       <c r="D4" t="s">
         <v>661</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>207555183118</v>
       </c>
       <c r="F4" t="s">
@@ -8824,7 +8832,7 @@
       <c r="D5" t="s">
         <v>666</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>208714677697</v>
       </c>
       <c r="F5" t="s">
@@ -8853,7 +8861,7 @@
       <c r="D6" t="s">
         <v>672</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>201564537686</v>
       </c>
       <c r="F6" t="s">

</xml_diff>

<commit_message>
Change the schema to be tried for acctg_db2
</commit_message>
<xml_diff>
--- a/db_tools/acctg_db1/acctg_export1.xlsx
+++ b/db_tools/acctg_db1/acctg_export1.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgrammingPython\thanos_app\db_tools\acctg_db1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914B8325-6071-4C1A-9E88-3A44BD8A50F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535865CF-AD9C-40F6-9FD8-71FC35F19D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="14" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="account_types" sheetId="1" r:id="rId1"/>
     <sheet name="accounts" sheetId="2" r:id="rId2"/>
-    <sheet name="contact_types" sheetId="3" r:id="rId3"/>
-    <sheet name="contacts" sheetId="4" r:id="rId4"/>
+    <sheet name="entity_types" sheetId="3" r:id="rId3"/>
+    <sheet name="entities" sheetId="4" r:id="rId4"/>
     <sheet name="fiscal_years" sheetId="5" r:id="rId5"/>
     <sheet name="users" sheetId="21" r:id="rId6"/>
     <sheet name="currencies" sheetId="6" r:id="rId7"/>
     <sheet name="tax_rates" sheetId="7" r:id="rId8"/>
     <sheet name="payment_methods" sheetId="8" r:id="rId9"/>
     <sheet name="bank_accounts" sheetId="9" r:id="rId10"/>
-    <sheet name="journal_entries" sheetId="10" r:id="rId11"/>
-    <sheet name="journal_entry_lines" sheetId="11" r:id="rId12"/>
+    <sheet name="journals" sheetId="10" r:id="rId11"/>
+    <sheet name="journal_lines" sheetId="11" r:id="rId12"/>
     <sheet name="product_categories" sheetId="12" r:id="rId13"/>
     <sheet name="products" sheetId="13" r:id="rId14"/>
     <sheet name="invoices" sheetId="14" r:id="rId15"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="682">
   <si>
     <t>id</t>
   </si>
@@ -1146,9 +1146,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>entry_number</t>
-  </si>
-  <si>
     <t>is_posted</t>
   </si>
   <si>
@@ -1899,9 +1896,6 @@
     <t>line_amount</t>
   </si>
   <si>
-    <t>contact_number</t>
-  </si>
-  <si>
     <t>C-123456</t>
   </si>
   <si>
@@ -2083,6 +2077,15 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>entity_number</t>
+  </si>
+  <si>
+    <t>journal_number</t>
+  </si>
+  <si>
+    <t>journal_id</t>
   </si>
 </sst>
 </file>
@@ -2141,16 +2144,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2691,7 +2690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2707,7 +2708,7 @@
         <v>367</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>368</v>
+        <v>680</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2716,7 +2717,7 @@
         <v>166</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>17</v>
@@ -2727,22 +2728,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2750,22 +2751,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2773,22 +2774,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2796,22 +2797,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2819,22 +2820,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2842,22 +2843,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2865,22 +2866,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -2888,22 +2889,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2911,22 +2912,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -2934,22 +2935,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -2957,22 +2958,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D12" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2980,22 +2981,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -3003,22 +3004,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -3026,22 +3027,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -3049,22 +3050,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E16" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -3072,22 +3073,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E17" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -3095,22 +3096,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D18" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E18" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -3118,22 +3119,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C19" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D19" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E19" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -3141,22 +3142,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D20" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E20" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -3164,22 +3165,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C21" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D21" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E21" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -3187,22 +3188,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C22" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D22" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E22" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -3210,22 +3211,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C23" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D23" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E23" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -3233,22 +3234,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D24" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E24" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -3256,22 +3257,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C25" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D25" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E25" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -3279,22 +3280,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C26" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D26" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E26" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -3302,22 +3303,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C27" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -3325,22 +3326,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C28" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E28" t="s">
+        <v>454</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
         <v>455</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" t="s">
-        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -3352,8 +3353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3370,7 +3371,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>457</v>
+        <v>681</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>354</v>
@@ -3379,10 +3380,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -3396,7 +3397,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E2">
         <v>50000</v>
@@ -3416,7 +3417,7 @@
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3436,7 +3437,7 @@
         <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E4">
         <v>2000</v>
@@ -3456,7 +3457,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3476,7 +3477,7 @@
         <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E6">
         <v>500</v>
@@ -3496,7 +3497,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -3516,7 +3517,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E8">
         <v>7500</v>
@@ -3536,7 +3537,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -3556,7 +3557,7 @@
         <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E10">
         <v>350</v>
@@ -3576,7 +3577,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -3596,7 +3597,7 @@
         <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E12">
         <v>12000</v>
@@ -3616,7 +3617,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -3636,7 +3637,7 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E14">
         <v>5000</v>
@@ -3656,7 +3657,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -3676,7 +3677,7 @@
         <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E16">
         <v>2000</v>
@@ -3696,7 +3697,7 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -3734,10 +3735,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3748,7 +3749,7 @@
         <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3756,10 +3757,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3767,10 +3768,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3778,10 +3779,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
   </sheetData>
@@ -3828,40 +3829,40 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>482</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>488</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>17</v>
@@ -3872,13 +3873,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3914,7 +3915,7 @@
         <v>37</v>
       </c>
       <c r="P2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -3922,13 +3923,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3964,7 +3965,7 @@
         <v>37</v>
       </c>
       <c r="P3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -3972,13 +3973,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -4014,7 +4015,7 @@
         <v>37</v>
       </c>
       <c r="P4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -4022,13 +4023,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -4064,7 +4065,7 @@
         <v>37</v>
       </c>
       <c r="P5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -4072,13 +4073,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -4114,7 +4115,7 @@
         <v>37</v>
       </c>
       <c r="P6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -4122,13 +4123,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -4164,7 +4165,7 @@
         <v>37</v>
       </c>
       <c r="P7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -4172,13 +4173,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C8" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D8" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -4205,7 +4206,7 @@
         <v>37</v>
       </c>
       <c r="P8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -4213,13 +4214,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -4246,7 +4247,7 @@
         <v>37</v>
       </c>
       <c r="P9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -4254,13 +4255,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C10" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D10" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -4287,7 +4288,7 @@
         <v>37</v>
       </c>
       <c r="P10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -4295,13 +4296,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C11" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D11" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -4337,7 +4338,7 @@
         <v>37</v>
       </c>
       <c r="P11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -4350,7 +4351,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4363,28 +4364,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>519</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>520</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>367</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>523</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>166</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>17</v>
@@ -4398,13 +4399,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F2">
         <v>2675</v>
@@ -4413,13 +4414,13 @@
         <v>175</v>
       </c>
       <c r="H2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -4430,13 +4431,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F3">
         <v>4815</v>
@@ -4445,13 +4446,13 @@
         <v>315</v>
       </c>
       <c r="H3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -4462,13 +4463,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F4">
         <v>1070</v>
@@ -4477,13 +4478,13 @@
         <v>70</v>
       </c>
       <c r="H4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -4494,13 +4495,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F5">
         <v>3210</v>
@@ -4509,13 +4510,13 @@
         <v>210</v>
       </c>
       <c r="H5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -4526,13 +4527,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F6">
         <v>5350</v>
@@ -4541,13 +4542,13 @@
         <v>350</v>
       </c>
       <c r="H6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -4558,13 +4559,13 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F7">
         <v>2140</v>
@@ -4573,13 +4574,13 @@
         <v>140</v>
       </c>
       <c r="H7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I7" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -4590,13 +4591,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D8" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E8" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F8">
         <v>3745</v>
@@ -4605,13 +4606,13 @@
         <v>245</v>
       </c>
       <c r="H8" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I8" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -4622,13 +4623,13 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F9">
         <v>1605</v>
@@ -4637,13 +4638,13 @@
         <v>105</v>
       </c>
       <c r="H9" t="s">
+        <v>547</v>
+      </c>
+      <c r="I9" t="s">
         <v>548</v>
       </c>
-      <c r="I9" t="s">
-        <v>549</v>
-      </c>
       <c r="J9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -4670,28 +4671,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>553</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -4705,7 +4706,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -4734,7 +4735,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -4763,7 +4764,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -4792,7 +4793,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -4821,7 +4822,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -4850,7 +4851,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -4879,7 +4880,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E8">
         <v>40</v>
@@ -4908,7 +4909,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -4937,7 +4938,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E10">
         <v>10</v>
@@ -4973,28 +4974,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>555</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>367</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>523</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>166</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>17</v>
@@ -5008,13 +5009,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F2">
         <v>535</v>
@@ -5023,13 +5024,13 @@
         <v>35</v>
       </c>
       <c r="H2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -5040,13 +5041,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F3">
         <v>3210</v>
@@ -5055,13 +5056,13 @@
         <v>210</v>
       </c>
       <c r="H3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -5072,13 +5073,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F4">
         <v>2140</v>
@@ -5087,13 +5088,13 @@
         <v>140</v>
       </c>
       <c r="H4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -5104,13 +5105,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F5">
         <v>1070</v>
@@ -5119,13 +5120,13 @@
         <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -5136,13 +5137,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F6">
         <v>428</v>
@@ -5151,13 +5152,13 @@
         <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -5168,13 +5169,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F7">
         <v>1605</v>
@@ -5183,13 +5184,13 @@
         <v>105</v>
       </c>
       <c r="H7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I7" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -5200,13 +5201,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D8" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E8" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F8">
         <v>2675</v>
@@ -5215,13 +5216,13 @@
         <v>175</v>
       </c>
       <c r="H8" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I8" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -5232,13 +5233,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F9">
         <v>3745</v>
@@ -5247,13 +5248,13 @@
         <v>245</v>
       </c>
       <c r="H9" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I9" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -5276,28 +5277,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>553</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -5311,7 +5312,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -5340,7 +5341,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -5369,7 +5370,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -5398,7 +5399,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -5427,7 +5428,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -5456,7 +5457,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -5485,7 +5486,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -5514,7 +5515,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E9">
         <v>40</v>
@@ -5543,7 +5544,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E10">
         <v>7</v>
@@ -5584,19 +5585,19 @@
         <v>367</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>572</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>573</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>166</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5604,7 +5605,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5613,10 +5614,10 @@
         <v>2675</v>
       </c>
       <c r="E2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -5627,7 +5628,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -5636,10 +5637,10 @@
         <v>4815</v>
       </c>
       <c r="E3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -5650,7 +5651,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -5659,10 +5660,10 @@
         <v>1070</v>
       </c>
       <c r="E4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -5673,7 +5674,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -5682,10 +5683,10 @@
         <v>3210</v>
       </c>
       <c r="E5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -5696,7 +5697,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -5705,10 +5706,10 @@
         <v>5350</v>
       </c>
       <c r="E6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -5719,7 +5720,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5728,10 +5729,10 @@
         <v>2140</v>
       </c>
       <c r="E7" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -5742,7 +5743,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -5751,10 +5752,10 @@
         <v>3745</v>
       </c>
       <c r="E8" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -5765,7 +5766,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -5774,10 +5775,10 @@
         <v>1605</v>
       </c>
       <c r="E9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -7036,19 +7037,19 @@
         <v>367</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>572</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>573</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>166</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -7056,7 +7057,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -7065,10 +7066,10 @@
         <v>535</v>
       </c>
       <c r="E2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -7079,7 +7080,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -7088,10 +7089,10 @@
         <v>3210</v>
       </c>
       <c r="E3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -7102,7 +7103,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -7111,10 +7112,10 @@
         <v>2140</v>
       </c>
       <c r="E4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -7125,7 +7126,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -7134,10 +7135,10 @@
         <v>1070</v>
       </c>
       <c r="E5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -7148,7 +7149,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -7157,10 +7158,10 @@
         <v>428</v>
       </c>
       <c r="E6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -7171,7 +7172,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -7180,10 +7181,10 @@
         <v>1605</v>
       </c>
       <c r="E7" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -7194,7 +7195,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -7203,10 +7204,10 @@
         <v>2675</v>
       </c>
       <c r="E8" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F8" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -7217,7 +7218,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -7226,10 +7227,10 @@
         <v>3745</v>
       </c>
       <c r="E9" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -7244,21 +7245,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="9" max="11" width="8.88671875" style="4"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>367</v>
@@ -7267,25 +7265,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>611</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -7299,25 +7297,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E2">
         <v>50000</v>
       </c>
       <c r="F2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -7328,25 +7326,25 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E3">
         <v>-2000</v>
       </c>
       <c r="F3" t="s">
+        <v>615</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
         <v>616</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="4">
-        <v>2</v>
-      </c>
-      <c r="L3" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -7357,25 +7355,25 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E4">
         <v>-500</v>
       </c>
       <c r="F4" t="s">
+        <v>615</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
         <v>616</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
-        <v>3</v>
-      </c>
-      <c r="L4" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -7386,25 +7384,25 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E5">
         <v>-535</v>
       </c>
       <c r="F5" t="s">
+        <v>615</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
         <v>616</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="4">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -7415,25 +7413,25 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E6">
         <v>7500</v>
       </c>
       <c r="F6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6">
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -7444,25 +7442,25 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E7">
         <v>2675</v>
       </c>
       <c r="F7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7">
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -7473,25 +7471,25 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E8">
         <v>-350</v>
       </c>
       <c r="F8" t="s">
+        <v>615</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="L8" t="s">
         <v>616</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="4">
-        <v>5</v>
-      </c>
-      <c r="L8" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -7502,25 +7500,25 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D9" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E9">
         <v>-3210</v>
       </c>
       <c r="F9" t="s">
+        <v>615</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
         <v>616</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="K9" s="4">
-        <v>2</v>
-      </c>
-      <c r="L9" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -7531,25 +7529,25 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E10">
         <v>4815</v>
       </c>
       <c r="F10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10">
         <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -7560,25 +7558,25 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E11">
         <v>-12000</v>
       </c>
       <c r="F11" t="s">
+        <v>615</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="L11" t="s">
         <v>616</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="4">
-        <v>6</v>
-      </c>
-      <c r="L11" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -7589,25 +7587,25 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E12">
         <v>-5000</v>
       </c>
       <c r="F12" t="s">
+        <v>615</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>7</v>
+      </c>
+      <c r="L12" t="s">
         <v>616</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="4">
-        <v>7</v>
-      </c>
-      <c r="L12" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -7618,25 +7616,25 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E13">
         <v>-2000</v>
       </c>
       <c r="F13" t="s">
+        <v>615</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="L13" t="s">
         <v>616</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13" s="4">
-        <v>8</v>
-      </c>
-      <c r="L13" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -7647,25 +7645,25 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D14" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E14">
         <v>-2140</v>
       </c>
       <c r="F14" t="s">
+        <v>615</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
+      <c r="L14" t="s">
         <v>616</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="K14" s="4">
-        <v>3</v>
-      </c>
-      <c r="L14" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -7676,25 +7674,25 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D15" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E15">
         <v>1070</v>
       </c>
       <c r="F15" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15">
         <v>3</v>
       </c>
       <c r="L15" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
   </sheetData>
@@ -7752,7 +7750,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7790,7 +7788,7 @@
         <v>156</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>619</v>
+        <v>679</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>157</v>
@@ -7843,7 +7841,7 @@
         <v>182</v>
       </c>
       <c r="E2" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F2" t="s">
         <v>191</v>
@@ -7896,7 +7894,7 @@
         <v>183</v>
       </c>
       <c r="E3" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="F3" t="s">
         <v>192</v>
@@ -7949,7 +7947,7 @@
         <v>184</v>
       </c>
       <c r="E4" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="F4" t="s">
         <v>193</v>
@@ -8002,7 +8000,7 @@
         <v>185</v>
       </c>
       <c r="E5" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F5" t="s">
         <v>194</v>
@@ -8055,7 +8053,7 @@
         <v>186</v>
       </c>
       <c r="E6" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F6" t="s">
         <v>195</v>
@@ -8111,7 +8109,7 @@
         <v>196</v>
       </c>
       <c r="F7" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="G7" t="s">
         <v>211</v>
@@ -8164,7 +8162,7 @@
         <v>197</v>
       </c>
       <c r="F8" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="G8" t="s">
         <v>212</v>
@@ -8217,7 +8215,7 @@
         <v>198</v>
       </c>
       <c r="F9" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G9" t="s">
         <v>213</v>
@@ -8270,7 +8268,7 @@
         <v>199</v>
       </c>
       <c r="F10" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="G10" t="s">
         <v>214</v>
@@ -8323,7 +8321,7 @@
         <v>200</v>
       </c>
       <c r="F11" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="G11" t="s">
         <v>215</v>
@@ -8370,13 +8368,13 @@
         <v>177</v>
       </c>
       <c r="D12" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E12" t="s">
         <v>201</v>
       </c>
       <c r="F12" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="G12" t="s">
         <v>216</v>
@@ -8397,10 +8395,10 @@
         <v>274</v>
       </c>
       <c r="M12" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="N12" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="O12" t="s">
         <v>309</v>
@@ -8423,13 +8421,13 @@
         <v>178</v>
       </c>
       <c r="D13" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E13" t="s">
         <v>202</v>
       </c>
       <c r="F13" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="G13" t="s">
         <v>217</v>
@@ -8450,10 +8448,10 @@
         <v>275</v>
       </c>
       <c r="M13" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="N13" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="O13" t="s">
         <v>310</v>
@@ -8476,13 +8474,13 @@
         <v>179</v>
       </c>
       <c r="D14" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E14" t="s">
         <v>203</v>
       </c>
       <c r="F14" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="G14" t="s">
         <v>218</v>
@@ -8503,10 +8501,10 @@
         <v>276</v>
       </c>
       <c r="M14" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="N14" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="O14" t="s">
         <v>311</v>
@@ -8529,13 +8527,13 @@
         <v>180</v>
       </c>
       <c r="D15" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E15" t="s">
         <v>204</v>
       </c>
       <c r="F15" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="G15" t="s">
         <v>219</v>
@@ -8556,10 +8554,10 @@
         <v>277</v>
       </c>
       <c r="M15" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="N15" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="O15" t="s">
         <v>312</v>
@@ -8582,13 +8580,13 @@
         <v>181</v>
       </c>
       <c r="D16" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E16" t="s">
         <v>205</v>
       </c>
       <c r="F16" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="G16" t="s">
         <v>220</v>
@@ -8609,10 +8607,10 @@
         <v>278</v>
       </c>
       <c r="M16" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="N16" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="O16" t="s">
         <v>313</v>
@@ -8708,28 +8706,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C1" t="s">
+        <v>641</v>
+      </c>
+      <c r="D1" t="s">
         <v>642</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="2" t="s">
         <v>643</v>
-      </c>
-      <c r="D1" t="s">
-        <v>644</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>645</v>
       </c>
       <c r="F1" t="s">
         <v>158</v>
       </c>
       <c r="G1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="H1" t="s">
         <v>164</v>
       </c>
       <c r="I1" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -8737,28 +8735,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>645</v>
+      </c>
+      <c r="C2" t="s">
+        <v>646</v>
+      </c>
+      <c r="D2" t="s">
         <v>647</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>648</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>649</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>651</v>
+      </c>
+      <c r="H2" t="s">
         <v>650</v>
       </c>
-      <c r="F2" t="s">
-        <v>651</v>
-      </c>
-      <c r="G2" t="s">
-        <v>653</v>
-      </c>
-      <c r="H2" t="s">
-        <v>652</v>
-      </c>
       <c r="I2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -8766,28 +8764,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C3" t="s">
+        <v>653</v>
+      </c>
+      <c r="D3" t="s">
         <v>654</v>
-      </c>
-      <c r="C3" t="s">
-        <v>655</v>
-      </c>
-      <c r="D3" t="s">
-        <v>656</v>
       </c>
       <c r="E3" s="2">
         <v>209268717220</v>
       </c>
       <c r="F3" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="G3" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="H3" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="I3" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -8795,28 +8793,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>657</v>
+      </c>
+      <c r="C4" t="s">
+        <v>658</v>
+      </c>
+      <c r="D4" t="s">
         <v>659</v>
-      </c>
-      <c r="C4" t="s">
-        <v>660</v>
-      </c>
-      <c r="D4" t="s">
-        <v>661</v>
       </c>
       <c r="E4" s="2">
         <v>207555183118</v>
       </c>
       <c r="F4" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="G4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="H4" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="I4" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -8824,28 +8822,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>662</v>
+      </c>
+      <c r="C5" t="s">
+        <v>663</v>
+      </c>
+      <c r="D5" t="s">
         <v>664</v>
-      </c>
-      <c r="C5" t="s">
-        <v>665</v>
-      </c>
-      <c r="D5" t="s">
-        <v>666</v>
       </c>
       <c r="E5" s="2">
         <v>208714677697</v>
       </c>
       <c r="F5" t="s">
+        <v>665</v>
+      </c>
+      <c r="G5" t="s">
         <v>667</v>
       </c>
-      <c r="G5" t="s">
-        <v>669</v>
-      </c>
       <c r="H5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="I5" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -8853,28 +8851,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>668</v>
+      </c>
+      <c r="C6" t="s">
+        <v>669</v>
+      </c>
+      <c r="D6" t="s">
         <v>670</v>
-      </c>
-      <c r="C6" t="s">
-        <v>671</v>
-      </c>
-      <c r="D6" t="s">
-        <v>672</v>
       </c>
       <c r="E6" s="2">
         <v>201564537686</v>
       </c>
       <c r="F6" t="s">
+        <v>671</v>
+      </c>
+      <c r="G6" t="s">
+        <v>667</v>
+      </c>
+      <c r="H6" t="s">
+        <v>672</v>
+      </c>
+      <c r="I6" t="s">
         <v>673</v>
-      </c>
-      <c r="G6" t="s">
-        <v>669</v>
-      </c>
-      <c r="H6" t="s">
-        <v>674</v>
-      </c>
-      <c r="I6" t="s">
-        <v>675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>